<commit_message>
Updated schematics to include a power jumper
</commit_message>
<xml_diff>
--- a/MidiAnySync/midianysync_bom.xlsx
+++ b/MidiAnySync/midianysync_bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/_home/_schemes/_Midi/MidiThru/MidiAnySync/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aokudrya/Documents/GitHub/Midi-boards/MidiAnySync/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EECB88E4-E8D4-9E41-8F9A-4F4EE29C9A0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C9D9EC-29B4-4F4F-8A66-19D779A8B4E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16400" xr2:uid="{BFF4FDEE-40B4-5B4F-A303-76B9208D6481}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{BFF4FDEE-40B4-5B4F-A303-76B9208D6481}"/>
   </bookViews>
   <sheets>
     <sheet name="midianysync" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="210">
   <si>
     <t>D</t>
   </si>
@@ -227,9 +227,6 @@
   </si>
   <si>
     <t>JP1</t>
-  </si>
-  <si>
-    <t>Pin_Headers:Pin_Header_Straight_1x03_Pitch2.54mm</t>
   </si>
   <si>
     <t>Dual jumper, normally closed</t>
@@ -1004,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI241"/>
+  <dimension ref="A1:AI240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1055,10 +1052,10 @@
         <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E1">
         <v>1</v>
@@ -1072,10 +1069,10 @@
         <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1083,7 +1080,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s">
         <v>24</v>
@@ -1092,7 +1089,7 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1100,7 +1097,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -1117,7 +1114,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B5" t="s">
         <v>20</v>
@@ -1148,7 +1145,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
@@ -1157,7 +1154,7 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1171,7 +1168,7 @@
         <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D8" t="s">
         <v>62</v>
@@ -1199,24 +1196,24 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>203</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>198</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>204</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -1225,15 +1222,15 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>199</v>
+        <v>40</v>
       </c>
       <c r="E11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>204</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -1242,41 +1239,38 @@
         <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>199</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>205</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="D13" t="s">
-        <v>200</v>
+        <v>59</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" t="s">
-        <v>59</v>
+        <v>200</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -1284,13 +1278,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>201</v>
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1298,16 +1295,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>76</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1315,36 +1312,42 @@
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="Q19" t="s">
+        <v>31</v>
+      </c>
+      <c r="R19" t="s">
+        <v>32</v>
+      </c>
+      <c r="S19">
+        <v>3</v>
+      </c>
+      <c r="U19" t="s">
+        <v>30</v>
+      </c>
+      <c r="V19" t="s">
+        <v>28</v>
+      </c>
+      <c r="W19" t="s">
+        <v>92</v>
+      </c>
+      <c r="X19" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.2">
@@ -1364,10 +1367,10 @@
         <v>28</v>
       </c>
       <c r="W20" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="X20" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.2">
@@ -1386,11 +1389,8 @@
       <c r="V21" t="s">
         <v>28</v>
       </c>
-      <c r="W21" t="s">
-        <v>95</v>
-      </c>
-      <c r="X21" t="s">
-        <v>32</v>
+      <c r="Y21" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.2">
@@ -1409,8 +1409,14 @@
       <c r="V22" t="s">
         <v>28</v>
       </c>
-      <c r="Y22" t="s">
-        <v>98</v>
+      <c r="Z22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA22">
+        <v>1</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.2">
@@ -1433,10 +1439,10 @@
         <v>8</v>
       </c>
       <c r="AA23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.2">
@@ -1459,10 +1465,10 @@
         <v>8</v>
       </c>
       <c r="AA24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.2">
@@ -1485,10 +1491,10 @@
         <v>8</v>
       </c>
       <c r="AA25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.2">
@@ -1511,36 +1517,33 @@
         <v>8</v>
       </c>
       <c r="AA26">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="Q27" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="R27" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="S27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U27" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="V27" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z27" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA27">
-        <v>5</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>96</v>
+        <v>8</v>
+      </c>
+      <c r="W27" t="s">
+        <v>92</v>
+      </c>
+      <c r="X27" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.2">
@@ -1560,7 +1563,7 @@
         <v>8</v>
       </c>
       <c r="W28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="X28" t="s">
         <v>26</v>
@@ -1582,11 +1585,8 @@
       <c r="V29" t="s">
         <v>8</v>
       </c>
-      <c r="W29" t="s">
-        <v>95</v>
-      </c>
-      <c r="X29" t="s">
-        <v>26</v>
+      <c r="Y29" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.2">
@@ -1605,8 +1605,14 @@
       <c r="V30" t="s">
         <v>8</v>
       </c>
-      <c r="Y30" t="s">
-        <v>99</v>
+      <c r="Z30" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA30">
+        <v>1</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.2">
@@ -1629,10 +1635,10 @@
         <v>8</v>
       </c>
       <c r="AA31">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.2">
@@ -1640,25 +1646,22 @@
         <v>11</v>
       </c>
       <c r="R32" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="S32">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U32" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="V32" t="s">
         <v>8</v>
       </c>
-      <c r="Z32" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA32">
-        <v>2</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>96</v>
+      <c r="W32" t="s">
+        <v>92</v>
+      </c>
+      <c r="X32" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="17:28" x14ac:dyDescent="0.2">
@@ -1678,10 +1681,10 @@
         <v>8</v>
       </c>
       <c r="W33" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="X33" t="s">
-        <v>100</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="17:28" x14ac:dyDescent="0.2">
@@ -1700,11 +1703,8 @@
       <c r="V34" t="s">
         <v>8</v>
       </c>
-      <c r="W34" t="s">
-        <v>95</v>
-      </c>
-      <c r="X34" t="s">
-        <v>52</v>
+      <c r="Y34" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="17:28" x14ac:dyDescent="0.2">
@@ -1723,8 +1723,14 @@
       <c r="V35" t="s">
         <v>8</v>
       </c>
-      <c r="Y35" t="s">
-        <v>101</v>
+      <c r="Z35">
+        <v>1</v>
+      </c>
+      <c r="AA35">
+        <v>1</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="17:28" x14ac:dyDescent="0.2">
@@ -1744,13 +1750,13 @@
         <v>8</v>
       </c>
       <c r="Z36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="17:28" x14ac:dyDescent="0.2">
@@ -1758,25 +1764,22 @@
         <v>11</v>
       </c>
       <c r="R37" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="S37">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U37" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="V37" t="s">
         <v>8</v>
       </c>
-      <c r="Z37">
-        <v>2</v>
-      </c>
-      <c r="AA37">
-        <v>2</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>96</v>
+      <c r="W37" t="s">
+        <v>92</v>
+      </c>
+      <c r="X37" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="17:28" x14ac:dyDescent="0.2">
@@ -1796,7 +1799,7 @@
         <v>8</v>
       </c>
       <c r="W38" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="X38" t="s">
         <v>0</v>
@@ -1818,11 +1821,8 @@
       <c r="V39" t="s">
         <v>8</v>
       </c>
-      <c r="W39" t="s">
-        <v>95</v>
-      </c>
-      <c r="X39" t="s">
-        <v>0</v>
+      <c r="Y39" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="17:28" x14ac:dyDescent="0.2">
@@ -1901,8 +1901,14 @@
       <c r="V43" t="s">
         <v>8</v>
       </c>
-      <c r="Y43" t="s">
+      <c r="Z43" t="s">
         <v>105</v>
+      </c>
+      <c r="AA43">
+        <v>1</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="17:28" x14ac:dyDescent="0.2">
@@ -1925,10 +1931,10 @@
         <v>106</v>
       </c>
       <c r="AA44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="17:28" x14ac:dyDescent="0.2">
@@ -1936,25 +1942,22 @@
         <v>11</v>
       </c>
       <c r="R45" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="S45">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U45" t="s">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="V45" t="s">
         <v>8</v>
       </c>
-      <c r="Z45" t="s">
+      <c r="W45" t="s">
+        <v>92</v>
+      </c>
+      <c r="X45" t="s">
         <v>107</v>
-      </c>
-      <c r="AA45">
-        <v>2</v>
-      </c>
-      <c r="AB45" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="46" spans="17:28" x14ac:dyDescent="0.2">
@@ -1962,22 +1965,22 @@
         <v>11</v>
       </c>
       <c r="R46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S46">
         <v>7</v>
       </c>
       <c r="U46" t="s">
+        <v>69</v>
+      </c>
+      <c r="V46" t="s">
+        <v>8</v>
+      </c>
+      <c r="W46" t="s">
+        <v>94</v>
+      </c>
+      <c r="X46" t="s">
         <v>70</v>
-      </c>
-      <c r="V46" t="s">
-        <v>8</v>
-      </c>
-      <c r="W46" t="s">
-        <v>93</v>
-      </c>
-      <c r="X46" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="47" spans="17:28" x14ac:dyDescent="0.2">
@@ -1985,22 +1988,25 @@
         <v>11</v>
       </c>
       <c r="R47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S47">
         <v>7</v>
       </c>
       <c r="U47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V47" t="s">
         <v>8</v>
       </c>
-      <c r="W47" t="s">
+      <c r="Z47">
+        <v>1</v>
+      </c>
+      <c r="AA47">
+        <v>1</v>
+      </c>
+      <c r="AB47" t="s">
         <v>95</v>
-      </c>
-      <c r="X47" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="48" spans="17:28" x14ac:dyDescent="0.2">
@@ -2008,25 +2014,25 @@
         <v>11</v>
       </c>
       <c r="R48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S48">
         <v>7</v>
       </c>
       <c r="U48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V48" t="s">
         <v>8</v>
       </c>
       <c r="Z48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB48" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="17:28" x14ac:dyDescent="0.2">
@@ -2034,25 +2040,25 @@
         <v>11</v>
       </c>
       <c r="R49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="S49">
         <v>7</v>
       </c>
       <c r="U49" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="V49" t="s">
         <v>8</v>
       </c>
       <c r="Z49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AA49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="17:28" x14ac:dyDescent="0.2">
@@ -2060,25 +2066,22 @@
         <v>11</v>
       </c>
       <c r="R50" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="S50">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="U50" t="s">
-        <v>70</v>
+        <v>21</v>
       </c>
       <c r="V50" t="s">
         <v>8</v>
       </c>
-      <c r="Z50">
-        <v>3</v>
-      </c>
-      <c r="AA50">
-        <v>3</v>
-      </c>
-      <c r="AB50" t="s">
-        <v>96</v>
+      <c r="W50" t="s">
+        <v>92</v>
+      </c>
+      <c r="X50" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="17:28" x14ac:dyDescent="0.2">
@@ -2098,10 +2101,10 @@
         <v>8</v>
       </c>
       <c r="W51" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="X51" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="52" spans="17:28" x14ac:dyDescent="0.2">
@@ -2120,11 +2123,8 @@
       <c r="V52" t="s">
         <v>8</v>
       </c>
-      <c r="W52" t="s">
-        <v>95</v>
-      </c>
-      <c r="X52" t="s">
-        <v>22</v>
+      <c r="Y52" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="17:28" x14ac:dyDescent="0.2">
@@ -2183,8 +2183,14 @@
       <c r="V55" t="s">
         <v>8</v>
       </c>
-      <c r="Y55" t="s">
-        <v>111</v>
+      <c r="Z55" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA55">
+        <v>1</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="17:28" x14ac:dyDescent="0.2">
@@ -2207,10 +2213,10 @@
         <v>106</v>
       </c>
       <c r="AA56">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="57" spans="17:28" x14ac:dyDescent="0.2">
@@ -2218,25 +2224,22 @@
         <v>11</v>
       </c>
       <c r="R57" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="S57">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U57" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="V57" t="s">
         <v>8</v>
       </c>
-      <c r="Z57" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA57">
-        <v>2</v>
-      </c>
-      <c r="AB57" t="s">
-        <v>96</v>
+      <c r="W57" t="s">
+        <v>92</v>
+      </c>
+      <c r="X57" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="17:28" x14ac:dyDescent="0.2">
@@ -2256,7 +2259,7 @@
         <v>8</v>
       </c>
       <c r="W58" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="X58" t="s">
         <v>12</v>
@@ -2278,11 +2281,8 @@
       <c r="V59" t="s">
         <v>8</v>
       </c>
-      <c r="W59" t="s">
-        <v>95</v>
-      </c>
-      <c r="X59" t="s">
-        <v>12</v>
+      <c r="Y59" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="17:28" x14ac:dyDescent="0.2">
@@ -2301,8 +2301,14 @@
       <c r="V60" t="s">
         <v>8</v>
       </c>
-      <c r="Y60" t="s">
-        <v>112</v>
+      <c r="Z60" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA60">
+        <v>1</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="61" spans="17:28" x14ac:dyDescent="0.2">
@@ -2325,36 +2331,36 @@
         <v>8</v>
       </c>
       <c r="AA61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB61" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q62" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="R62" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="S62">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="T62" t="s">
+        <v>112</v>
       </c>
       <c r="U62" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="V62" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z62" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA62">
         <v>2</v>
       </c>
-      <c r="AB62" t="s">
-        <v>96</v>
+      <c r="W62" t="s">
+        <v>92</v>
+      </c>
+      <c r="X62" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="17:28" x14ac:dyDescent="0.2">
@@ -2368,7 +2374,7 @@
         <v>10</v>
       </c>
       <c r="T63" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U63" t="s">
         <v>4</v>
@@ -2377,10 +2383,10 @@
         <v>2</v>
       </c>
       <c r="W63" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="X63" t="s">
-        <v>94</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="17:28" x14ac:dyDescent="0.2">
@@ -2394,7 +2400,7 @@
         <v>10</v>
       </c>
       <c r="T64" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U64" t="s">
         <v>4</v>
@@ -2402,11 +2408,8 @@
       <c r="V64" t="s">
         <v>2</v>
       </c>
-      <c r="W64" t="s">
-        <v>95</v>
-      </c>
-      <c r="X64" t="s">
-        <v>6</v>
+      <c r="Y64" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="65" spans="17:28" x14ac:dyDescent="0.2">
@@ -2420,7 +2423,7 @@
         <v>10</v>
       </c>
       <c r="T65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U65" t="s">
         <v>4</v>
@@ -2443,7 +2446,7 @@
         <v>10</v>
       </c>
       <c r="T66" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U66" t="s">
         <v>4</v>
@@ -2451,8 +2454,14 @@
       <c r="V66" t="s">
         <v>2</v>
       </c>
-      <c r="Y66" t="s">
+      <c r="Z66" t="s">
         <v>115</v>
+      </c>
+      <c r="AA66">
+        <v>1</v>
+      </c>
+      <c r="AB66" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="17:28" x14ac:dyDescent="0.2">
@@ -2466,7 +2475,7 @@
         <v>10</v>
       </c>
       <c r="T67" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U67" t="s">
         <v>4</v>
@@ -2475,13 +2484,13 @@
         <v>2</v>
       </c>
       <c r="Z67" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="AA67">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB67" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
     </row>
     <row r="68" spans="17:28" x14ac:dyDescent="0.2">
@@ -2495,7 +2504,7 @@
         <v>10</v>
       </c>
       <c r="T68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U68" t="s">
         <v>4</v>
@@ -2504,13 +2513,13 @@
         <v>2</v>
       </c>
       <c r="Z68" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="AA68">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB68" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="17:28" x14ac:dyDescent="0.2">
@@ -2524,7 +2533,7 @@
         <v>10</v>
       </c>
       <c r="T69" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U69" t="s">
         <v>4</v>
@@ -2533,13 +2542,13 @@
         <v>2</v>
       </c>
       <c r="Z69" t="s">
-        <v>37</v>
+        <v>115</v>
       </c>
       <c r="AA69">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB69" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
     </row>
     <row r="70" spans="17:28" x14ac:dyDescent="0.2">
@@ -2553,7 +2562,7 @@
         <v>10</v>
       </c>
       <c r="T70" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U70" t="s">
         <v>4</v>
@@ -2562,13 +2571,13 @@
         <v>2</v>
       </c>
       <c r="Z70" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="AA70">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB70" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
     </row>
     <row r="71" spans="17:28" x14ac:dyDescent="0.2">
@@ -2582,7 +2591,7 @@
         <v>10</v>
       </c>
       <c r="T71" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U71" t="s">
         <v>4</v>
@@ -2594,10 +2603,10 @@
         <v>118</v>
       </c>
       <c r="AA71">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AB71" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="72" spans="17:28" x14ac:dyDescent="0.2">
@@ -2611,7 +2620,7 @@
         <v>10</v>
       </c>
       <c r="T72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U72" t="s">
         <v>4</v>
@@ -2623,10 +2632,10 @@
         <v>119</v>
       </c>
       <c r="AA72">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AB72" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="73" spans="17:28" x14ac:dyDescent="0.2">
@@ -2640,7 +2649,7 @@
         <v>10</v>
       </c>
       <c r="T73" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U73" t="s">
         <v>4</v>
@@ -2652,39 +2661,36 @@
         <v>120</v>
       </c>
       <c r="AA73">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q74" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="R74" t="s">
-        <v>6</v>
+        <v>121</v>
       </c>
       <c r="S74">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="T74" t="s">
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="U74" t="s">
-        <v>4</v>
+        <v>122</v>
       </c>
       <c r="V74" t="s">
-        <v>2</v>
-      </c>
-      <c r="Z74" t="s">
-        <v>121</v>
-      </c>
-      <c r="AA74">
-        <v>8</v>
-      </c>
-      <c r="AB74" t="s">
-        <v>96</v>
+        <v>42</v>
+      </c>
+      <c r="W74" t="s">
+        <v>92</v>
+      </c>
+      <c r="X74" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="75" spans="17:28" x14ac:dyDescent="0.2">
@@ -2692,7 +2698,7 @@
         <v>44</v>
       </c>
       <c r="R75" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S75">
         <v>11</v>
@@ -2701,16 +2707,16 @@
         <v>45</v>
       </c>
       <c r="U75" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V75" t="s">
         <v>42</v>
       </c>
       <c r="W75" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="X75" t="s">
-        <v>94</v>
+        <v>121</v>
       </c>
     </row>
     <row r="76" spans="17:28" x14ac:dyDescent="0.2">
@@ -2718,7 +2724,7 @@
         <v>44</v>
       </c>
       <c r="R76" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S76">
         <v>11</v>
@@ -2727,16 +2733,13 @@
         <v>45</v>
       </c>
       <c r="U76" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V76" t="s">
         <v>42</v>
       </c>
-      <c r="W76" t="s">
-        <v>95</v>
-      </c>
-      <c r="X76" t="s">
-        <v>122</v>
+      <c r="Y76" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="77" spans="17:28" x14ac:dyDescent="0.2">
@@ -2744,7 +2747,7 @@
         <v>44</v>
       </c>
       <c r="R77" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S77">
         <v>11</v>
@@ -2753,7 +2756,7 @@
         <v>45</v>
       </c>
       <c r="U77" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V77" t="s">
         <v>42</v>
@@ -2767,7 +2770,7 @@
         <v>44</v>
       </c>
       <c r="R78" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S78">
         <v>11</v>
@@ -2776,13 +2779,19 @@
         <v>45</v>
       </c>
       <c r="U78" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V78" t="s">
         <v>42</v>
       </c>
-      <c r="Y78" t="s">
+      <c r="Z78" t="s">
         <v>125</v>
+      </c>
+      <c r="AA78">
+        <v>1</v>
+      </c>
+      <c r="AB78" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="79" spans="17:28" x14ac:dyDescent="0.2">
@@ -2790,7 +2799,7 @@
         <v>44</v>
       </c>
       <c r="R79" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S79">
         <v>11</v>
@@ -2799,19 +2808,19 @@
         <v>45</v>
       </c>
       <c r="U79" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V79" t="s">
         <v>42</v>
       </c>
       <c r="Z79" t="s">
+        <v>127</v>
+      </c>
+      <c r="AA79">
+        <v>2</v>
+      </c>
+      <c r="AB79" t="s">
         <v>126</v>
-      </c>
-      <c r="AA79">
-        <v>1</v>
-      </c>
-      <c r="AB79" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="80" spans="17:28" x14ac:dyDescent="0.2">
@@ -2819,7 +2828,7 @@
         <v>44</v>
       </c>
       <c r="R80" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S80">
         <v>11</v>
@@ -2828,7 +2837,7 @@
         <v>45</v>
       </c>
       <c r="U80" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V80" t="s">
         <v>42</v>
@@ -2837,10 +2846,10 @@
         <v>128</v>
       </c>
       <c r="AA80">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB80" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="81" spans="17:28" x14ac:dyDescent="0.2">
@@ -2848,7 +2857,7 @@
         <v>44</v>
       </c>
       <c r="R81" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S81">
         <v>11</v>
@@ -2857,7 +2866,7 @@
         <v>45</v>
       </c>
       <c r="U81" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V81" t="s">
         <v>42</v>
@@ -2866,10 +2875,10 @@
         <v>129</v>
       </c>
       <c r="AA81">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB81" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="82" spans="17:28" x14ac:dyDescent="0.2">
@@ -2877,7 +2886,7 @@
         <v>44</v>
       </c>
       <c r="R82" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S82">
         <v>11</v>
@@ -2886,19 +2895,19 @@
         <v>45</v>
       </c>
       <c r="U82" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V82" t="s">
         <v>42</v>
       </c>
       <c r="Z82" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="AA82">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB82" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="17:28" x14ac:dyDescent="0.2">
@@ -2906,7 +2915,7 @@
         <v>44</v>
       </c>
       <c r="R83" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S83">
         <v>11</v>
@@ -2915,19 +2924,19 @@
         <v>45</v>
       </c>
       <c r="U83" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V83" t="s">
         <v>42</v>
       </c>
       <c r="Z83" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="AA83">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AB83" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="84" spans="17:28" x14ac:dyDescent="0.2">
@@ -2935,7 +2944,7 @@
         <v>44</v>
       </c>
       <c r="R84" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S84">
         <v>11</v>
@@ -2944,7 +2953,7 @@
         <v>45</v>
       </c>
       <c r="U84" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V84" t="s">
         <v>42</v>
@@ -2953,10 +2962,10 @@
         <v>134</v>
       </c>
       <c r="AA84">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AB84" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="85" spans="17:28" x14ac:dyDescent="0.2">
@@ -2964,7 +2973,7 @@
         <v>44</v>
       </c>
       <c r="R85" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S85">
         <v>11</v>
@@ -2973,7 +2982,7 @@
         <v>45</v>
       </c>
       <c r="U85" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V85" t="s">
         <v>42</v>
@@ -2982,10 +2991,10 @@
         <v>135</v>
       </c>
       <c r="AA85">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB85" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="86" spans="17:28" x14ac:dyDescent="0.2">
@@ -2993,7 +3002,7 @@
         <v>44</v>
       </c>
       <c r="R86" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S86">
         <v>11</v>
@@ -3002,7 +3011,7 @@
         <v>45</v>
       </c>
       <c r="U86" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V86" t="s">
         <v>42</v>
@@ -3011,10 +3020,10 @@
         <v>136</v>
       </c>
       <c r="AA86">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AB86" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="87" spans="17:28" x14ac:dyDescent="0.2">
@@ -3022,7 +3031,7 @@
         <v>44</v>
       </c>
       <c r="R87" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S87">
         <v>11</v>
@@ -3031,7 +3040,7 @@
         <v>45</v>
       </c>
       <c r="U87" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V87" t="s">
         <v>42</v>
@@ -3040,10 +3049,10 @@
         <v>137</v>
       </c>
       <c r="AA87">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AB87" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="88" spans="17:28" x14ac:dyDescent="0.2">
@@ -3051,7 +3060,7 @@
         <v>44</v>
       </c>
       <c r="R88" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S88">
         <v>11</v>
@@ -3060,7 +3069,7 @@
         <v>45</v>
       </c>
       <c r="U88" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V88" t="s">
         <v>42</v>
@@ -3069,10 +3078,10 @@
         <v>138</v>
       </c>
       <c r="AA88">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AB88" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="89" spans="17:28" x14ac:dyDescent="0.2">
@@ -3080,7 +3089,7 @@
         <v>44</v>
       </c>
       <c r="R89" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S89">
         <v>11</v>
@@ -3089,7 +3098,7 @@
         <v>45</v>
       </c>
       <c r="U89" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V89" t="s">
         <v>42</v>
@@ -3098,10 +3107,10 @@
         <v>139</v>
       </c>
       <c r="AA89">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AB89" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="90" spans="17:28" x14ac:dyDescent="0.2">
@@ -3109,7 +3118,7 @@
         <v>44</v>
       </c>
       <c r="R90" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S90">
         <v>11</v>
@@ -3118,7 +3127,7 @@
         <v>45</v>
       </c>
       <c r="U90" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V90" t="s">
         <v>42</v>
@@ -3127,10 +3136,10 @@
         <v>140</v>
       </c>
       <c r="AA90">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AB90" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="91" spans="17:28" x14ac:dyDescent="0.2">
@@ -3138,7 +3147,7 @@
         <v>44</v>
       </c>
       <c r="R91" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S91">
         <v>11</v>
@@ -3147,7 +3156,7 @@
         <v>45</v>
       </c>
       <c r="U91" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V91" t="s">
         <v>42</v>
@@ -3156,10 +3165,10 @@
         <v>141</v>
       </c>
       <c r="AA91">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AB91" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="92" spans="17:28" x14ac:dyDescent="0.2">
@@ -3167,7 +3176,7 @@
         <v>44</v>
       </c>
       <c r="R92" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S92">
         <v>11</v>
@@ -3176,7 +3185,7 @@
         <v>45</v>
       </c>
       <c r="U92" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V92" t="s">
         <v>42</v>
@@ -3185,10 +3194,10 @@
         <v>142</v>
       </c>
       <c r="AA92">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB92" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="17:28" x14ac:dyDescent="0.2">
@@ -3196,7 +3205,7 @@
         <v>44</v>
       </c>
       <c r="R93" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S93">
         <v>11</v>
@@ -3205,19 +3214,19 @@
         <v>45</v>
       </c>
       <c r="U93" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V93" t="s">
         <v>42</v>
       </c>
       <c r="Z93" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AA93">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AB93" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="94" spans="17:28" x14ac:dyDescent="0.2">
@@ -3225,7 +3234,7 @@
         <v>44</v>
       </c>
       <c r="R94" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S94">
         <v>11</v>
@@ -3234,7 +3243,7 @@
         <v>45</v>
       </c>
       <c r="U94" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V94" t="s">
         <v>42</v>
@@ -3243,10 +3252,10 @@
         <v>145</v>
       </c>
       <c r="AA94">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AB94" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="95" spans="17:28" x14ac:dyDescent="0.2">
@@ -3254,7 +3263,7 @@
         <v>44</v>
       </c>
       <c r="R95" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S95">
         <v>11</v>
@@ -3263,7 +3272,7 @@
         <v>45</v>
       </c>
       <c r="U95" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V95" t="s">
         <v>42</v>
@@ -3272,39 +3281,30 @@
         <v>146</v>
       </c>
       <c r="AA95">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AB95" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="96" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q96" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="R96" t="s">
-        <v>122</v>
+        <v>58</v>
       </c>
       <c r="S96">
-        <v>11</v>
-      </c>
-      <c r="T96" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="U96" t="s">
-        <v>123</v>
-      </c>
-      <c r="V96" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z96" t="s">
+        <v>56</v>
+      </c>
+      <c r="W96" t="s">
+        <v>92</v>
+      </c>
+      <c r="X96" t="s">
         <v>147</v>
-      </c>
-      <c r="AA96">
-        <v>18</v>
-      </c>
-      <c r="AB96" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="97" spans="17:28" x14ac:dyDescent="0.2">
@@ -3321,10 +3321,10 @@
         <v>56</v>
       </c>
       <c r="W97" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="X97" t="s">
-        <v>148</v>
+        <v>58</v>
       </c>
     </row>
     <row r="98" spans="17:28" x14ac:dyDescent="0.2">
@@ -3340,11 +3340,8 @@
       <c r="U98" t="s">
         <v>56</v>
       </c>
-      <c r="W98" t="s">
-        <v>95</v>
-      </c>
-      <c r="X98" t="s">
-        <v>58</v>
+      <c r="Y98" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="99" spans="17:28" x14ac:dyDescent="0.2">
@@ -3360,8 +3357,14 @@
       <c r="U99" t="s">
         <v>56</v>
       </c>
-      <c r="Y99" t="s">
-        <v>149</v>
+      <c r="Z99" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA99">
+        <v>1</v>
+      </c>
+      <c r="AB99" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="100" spans="17:28" x14ac:dyDescent="0.2">
@@ -3381,10 +3384,10 @@
         <v>8</v>
       </c>
       <c r="AA100">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB100" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="101" spans="17:28" x14ac:dyDescent="0.2">
@@ -3404,10 +3407,10 @@
         <v>8</v>
       </c>
       <c r="AA101">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB101" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="102" spans="17:28" x14ac:dyDescent="0.2">
@@ -3427,10 +3430,10 @@
         <v>8</v>
       </c>
       <c r="AA102">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB102" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="17:28" x14ac:dyDescent="0.2">
@@ -3450,10 +3453,10 @@
         <v>8</v>
       </c>
       <c r="AA103">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AB103" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="104" spans="17:28" x14ac:dyDescent="0.2">
@@ -3473,10 +3476,10 @@
         <v>8</v>
       </c>
       <c r="AA104">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AB104" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="105" spans="17:28" x14ac:dyDescent="0.2">
@@ -3496,10 +3499,10 @@
         <v>8</v>
       </c>
       <c r="AA105">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AB105" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="106" spans="17:28" x14ac:dyDescent="0.2">
@@ -3519,10 +3522,10 @@
         <v>8</v>
       </c>
       <c r="AA106">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AB106" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="107" spans="17:28" x14ac:dyDescent="0.2">
@@ -3542,10 +3545,10 @@
         <v>8</v>
       </c>
       <c r="AA107">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AB107" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="108" spans="17:28" x14ac:dyDescent="0.2">
@@ -3565,10 +3568,10 @@
         <v>8</v>
       </c>
       <c r="AA108">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AB108" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="109" spans="17:28" x14ac:dyDescent="0.2">
@@ -3588,10 +3591,10 @@
         <v>8</v>
       </c>
       <c r="AA109">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AB109" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="110" spans="17:28" x14ac:dyDescent="0.2">
@@ -3611,10 +3614,10 @@
         <v>8</v>
       </c>
       <c r="AA110">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AB110" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="111" spans="17:28" x14ac:dyDescent="0.2">
@@ -3634,10 +3637,10 @@
         <v>8</v>
       </c>
       <c r="AA111">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AB111" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="112" spans="17:28" x14ac:dyDescent="0.2">
@@ -3657,10 +3660,10 @@
         <v>8</v>
       </c>
       <c r="AA112">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AB112" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="113" spans="17:28" x14ac:dyDescent="0.2">
@@ -3680,10 +3683,10 @@
         <v>8</v>
       </c>
       <c r="AA113">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AB113" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="114" spans="17:28" x14ac:dyDescent="0.2">
@@ -3703,10 +3706,10 @@
         <v>8</v>
       </c>
       <c r="AA114">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AB114" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="115" spans="17:28" x14ac:dyDescent="0.2">
@@ -3726,10 +3729,10 @@
         <v>8</v>
       </c>
       <c r="AA115">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AB115" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="116" spans="17:28" x14ac:dyDescent="0.2">
@@ -3749,10 +3752,10 @@
         <v>8</v>
       </c>
       <c r="AA116">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AB116" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="117" spans="17:28" x14ac:dyDescent="0.2">
@@ -3772,10 +3775,10 @@
         <v>8</v>
       </c>
       <c r="AA117">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AB117" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="118" spans="17:28" x14ac:dyDescent="0.2">
@@ -3795,415 +3798,400 @@
         <v>8</v>
       </c>
       <c r="AA118">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AB118" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="119" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q119" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="R119" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="S119">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="U119" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z119" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA119">
-        <v>20</v>
-      </c>
-      <c r="AB119" t="s">
-        <v>96</v>
+        <v>76</v>
+      </c>
+      <c r="V119" t="s">
+        <v>72</v>
+      </c>
+      <c r="W119" t="s">
+        <v>92</v>
+      </c>
+      <c r="X119" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="120" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q120" t="s">
+        <v>77</v>
+      </c>
+      <c r="R120" t="s">
         <v>78</v>
-      </c>
-      <c r="R120" t="s">
-        <v>79</v>
       </c>
       <c r="S120">
         <v>13</v>
       </c>
       <c r="U120" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V120" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W120" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="X120" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="121" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q121" t="s">
+        <v>77</v>
+      </c>
+      <c r="R121" t="s">
         <v>78</v>
-      </c>
-      <c r="R121" t="s">
-        <v>79</v>
       </c>
       <c r="S121">
         <v>13</v>
       </c>
       <c r="U121" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V121" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W121" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
       <c r="X121" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
     </row>
     <row r="122" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q122" t="s">
+        <v>77</v>
+      </c>
+      <c r="R122" t="s">
         <v>78</v>
-      </c>
-      <c r="R122" t="s">
-        <v>79</v>
       </c>
       <c r="S122">
         <v>13</v>
       </c>
       <c r="U122" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V122" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W122" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="X122" t="s">
-        <v>151</v>
+        <v>72</v>
       </c>
     </row>
     <row r="123" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q123" t="s">
+        <v>77</v>
+      </c>
+      <c r="R123" t="s">
         <v>78</v>
-      </c>
-      <c r="R123" t="s">
-        <v>79</v>
       </c>
       <c r="S123">
         <v>13</v>
       </c>
       <c r="U123" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V123" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W123" t="s">
-        <v>152</v>
+        <v>83</v>
       </c>
       <c r="X123" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
     </row>
     <row r="124" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q124" t="s">
+        <v>77</v>
+      </c>
+      <c r="R124" t="s">
         <v>78</v>
-      </c>
-      <c r="R124" t="s">
-        <v>79</v>
       </c>
       <c r="S124">
         <v>13</v>
       </c>
       <c r="U124" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V124" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W124" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="X124" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="125" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q125" t="s">
+        <v>77</v>
+      </c>
+      <c r="R125" t="s">
         <v>78</v>
-      </c>
-      <c r="R125" t="s">
-        <v>79</v>
       </c>
       <c r="S125">
         <v>13</v>
       </c>
       <c r="U125" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V125" t="s">
+        <v>72</v>
+      </c>
+      <c r="W125" t="s">
         <v>73</v>
       </c>
-      <c r="W125" t="s">
-        <v>88</v>
-      </c>
       <c r="X125" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="126" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q126" t="s">
+        <v>77</v>
+      </c>
+      <c r="R126" t="s">
         <v>78</v>
-      </c>
-      <c r="R126" t="s">
-        <v>79</v>
       </c>
       <c r="S126">
         <v>13</v>
       </c>
       <c r="U126" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V126" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W126" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="X126" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
     </row>
     <row r="127" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q127" t="s">
+        <v>77</v>
+      </c>
+      <c r="R127" t="s">
         <v>78</v>
-      </c>
-      <c r="R127" t="s">
-        <v>79</v>
       </c>
       <c r="S127">
         <v>13</v>
       </c>
       <c r="U127" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V127" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W127" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="X127" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="128" spans="17:28" x14ac:dyDescent="0.2">
       <c r="Q128" t="s">
+        <v>77</v>
+      </c>
+      <c r="R128" t="s">
         <v>78</v>
-      </c>
-      <c r="R128" t="s">
-        <v>79</v>
       </c>
       <c r="S128">
         <v>13</v>
       </c>
       <c r="U128" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V128" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W128" t="s">
         <v>80</v>
       </c>
       <c r="X128" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="129" spans="17:35" x14ac:dyDescent="0.2">
       <c r="Q129" t="s">
+        <v>77</v>
+      </c>
+      <c r="R129" t="s">
         <v>78</v>
-      </c>
-      <c r="R129" t="s">
-        <v>79</v>
       </c>
       <c r="S129">
         <v>13</v>
       </c>
       <c r="U129" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V129" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W129" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="X129" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="130" spans="17:35" x14ac:dyDescent="0.2">
       <c r="Q130" t="s">
+        <v>77</v>
+      </c>
+      <c r="R130" t="s">
         <v>78</v>
-      </c>
-      <c r="R130" t="s">
-        <v>79</v>
       </c>
       <c r="S130">
         <v>13</v>
       </c>
       <c r="U130" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V130" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W130" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="X130" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
     <row r="131" spans="17:35" x14ac:dyDescent="0.2">
       <c r="Q131" t="s">
+        <v>77</v>
+      </c>
+      <c r="R131" t="s">
         <v>78</v>
-      </c>
-      <c r="R131" t="s">
-        <v>79</v>
       </c>
       <c r="S131">
         <v>13</v>
       </c>
       <c r="U131" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V131" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="W131" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="X131" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="132" spans="17:35" x14ac:dyDescent="0.2">
       <c r="Q132" t="s">
+        <v>77</v>
+      </c>
+      <c r="R132" t="s">
         <v>78</v>
-      </c>
-      <c r="R132" t="s">
-        <v>79</v>
       </c>
       <c r="S132">
         <v>13</v>
       </c>
       <c r="U132" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V132" t="s">
-        <v>73</v>
-      </c>
-      <c r="W132" t="s">
-        <v>91</v>
-      </c>
-      <c r="X132" t="s">
-        <v>92</v>
+        <v>72</v>
+      </c>
+      <c r="Z132" t="s">
+        <v>152</v>
+      </c>
+      <c r="AA132">
+        <v>1</v>
+      </c>
+      <c r="AB132" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="17:35" x14ac:dyDescent="0.2">
       <c r="Q133" t="s">
+        <v>77</v>
+      </c>
+      <c r="R133" t="s">
         <v>78</v>
-      </c>
-      <c r="R133" t="s">
-        <v>79</v>
       </c>
       <c r="S133">
         <v>13</v>
       </c>
       <c r="U133" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V133" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Z133" t="s">
-        <v>153</v>
+        <v>117</v>
       </c>
       <c r="AA133">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB133" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="134" spans="17:35" x14ac:dyDescent="0.2">
       <c r="Q134" t="s">
+        <v>77</v>
+      </c>
+      <c r="R134" t="s">
         <v>78</v>
-      </c>
-      <c r="R134" t="s">
-        <v>79</v>
       </c>
       <c r="S134">
         <v>13</v>
       </c>
       <c r="U134" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V134" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Z134" t="s">
-        <v>118</v>
+        <v>153</v>
       </c>
       <c r="AA134">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB134" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
     </row>
     <row r="135" spans="17:35" x14ac:dyDescent="0.2">
-      <c r="Q135" t="s">
-        <v>78</v>
-      </c>
-      <c r="R135" t="s">
-        <v>79</v>
-      </c>
-      <c r="S135">
-        <v>13</v>
-      </c>
-      <c r="U135" t="s">
-        <v>77</v>
-      </c>
-      <c r="V135" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z135" t="s">
-        <v>154</v>
-      </c>
-      <c r="AA135">
-        <v>3</v>
-      </c>
-      <c r="AB135" t="s">
+      <c r="AC135" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD135" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="136" spans="17:35" x14ac:dyDescent="0.2">
       <c r="AC136" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="AD136" t="s">
         <v>156</v>
@@ -4211,7 +4199,7 @@
     </row>
     <row r="137" spans="17:35" x14ac:dyDescent="0.2">
       <c r="AC137" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="AD137" t="s">
         <v>157</v>
@@ -4219,7 +4207,7 @@
     </row>
     <row r="138" spans="17:35" x14ac:dyDescent="0.2">
       <c r="AC138" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="AD138" t="s">
         <v>158</v>
@@ -4227,7 +4215,7 @@
     </row>
     <row r="139" spans="17:35" x14ac:dyDescent="0.2">
       <c r="AC139" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="AD139" t="s">
         <v>159</v>
@@ -4235,18 +4223,27 @@
     </row>
     <row r="140" spans="17:35" x14ac:dyDescent="0.2">
       <c r="AC140" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="AD140" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="141" spans="17:35" x14ac:dyDescent="0.2">
-      <c r="AC141" t="s">
-        <v>78</v>
-      </c>
-      <c r="AD141" t="s">
+      <c r="AE141">
+        <v>1</v>
+      </c>
+      <c r="AF141" t="s">
         <v>161</v>
+      </c>
+      <c r="AG141">
+        <v>1</v>
+      </c>
+      <c r="AH141">
+        <v>2</v>
+      </c>
+      <c r="AI141" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="142" spans="17:35" x14ac:dyDescent="0.2">
@@ -4254,16 +4251,16 @@
         <v>1</v>
       </c>
       <c r="AF142" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG142">
         <v>1</v>
       </c>
       <c r="AH142">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="AI142" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
     </row>
     <row r="143" spans="17:35" x14ac:dyDescent="0.2">
@@ -4271,16 +4268,16 @@
         <v>1</v>
       </c>
       <c r="AF143" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG143">
         <v>1</v>
       </c>
       <c r="AH143">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="AI143" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="17:35" x14ac:dyDescent="0.2">
@@ -4288,16 +4285,16 @@
         <v>1</v>
       </c>
       <c r="AF144" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG144">
         <v>1</v>
       </c>
       <c r="AH144">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="AI144" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="145" spans="31:35" x14ac:dyDescent="0.2">
@@ -4305,7 +4302,7 @@
         <v>1</v>
       </c>
       <c r="AF145" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG145">
         <v>1</v>
@@ -4314,7 +4311,7 @@
         <v>1</v>
       </c>
       <c r="AI145" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="146" spans="31:35" x14ac:dyDescent="0.2">
@@ -4322,7 +4319,7 @@
         <v>1</v>
       </c>
       <c r="AF146" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG146">
         <v>1</v>
@@ -4331,7 +4328,7 @@
         <v>1</v>
       </c>
       <c r="AI146" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="147" spans="31:35" x14ac:dyDescent="0.2">
@@ -4339,7 +4336,7 @@
         <v>1</v>
       </c>
       <c r="AF147" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG147">
         <v>1</v>
@@ -4348,7 +4345,7 @@
         <v>1</v>
       </c>
       <c r="AI147" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="148" spans="31:35" x14ac:dyDescent="0.2">
@@ -4356,7 +4353,7 @@
         <v>1</v>
       </c>
       <c r="AF148" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG148">
         <v>1</v>
@@ -4365,7 +4362,7 @@
         <v>1</v>
       </c>
       <c r="AI148" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="149" spans="31:35" x14ac:dyDescent="0.2">
@@ -4373,50 +4370,50 @@
         <v>1</v>
       </c>
       <c r="AF149" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AG149">
         <v>1</v>
       </c>
       <c r="AH149">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AI149" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="150" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE150">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AF150" t="s">
         <v>162</v>
       </c>
       <c r="AG150">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH150">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AI150" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE151">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF151" t="s">
         <v>163</v>
       </c>
       <c r="AG151">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH151">
         <v>1</v>
       </c>
       <c r="AI151" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="152" spans="31:35" x14ac:dyDescent="0.2">
@@ -4424,16 +4421,16 @@
         <v>3</v>
       </c>
       <c r="AF152" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AG152">
         <v>3</v>
       </c>
       <c r="AH152">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI152" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="31:35" x14ac:dyDescent="0.2">
@@ -4441,50 +4438,50 @@
         <v>3</v>
       </c>
       <c r="AF153" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="AG153">
         <v>3</v>
       </c>
       <c r="AH153">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI153" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="154" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE154">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AF154" t="s">
         <v>164</v>
       </c>
       <c r="AG154">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH154">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AI154" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE155">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF155" t="s">
         <v>165</v>
       </c>
       <c r="AG155">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH155">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AI155" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="156" spans="31:35" x14ac:dyDescent="0.2">
@@ -4492,7 +4489,7 @@
         <v>5</v>
       </c>
       <c r="AF156" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AG156">
         <v>5</v>
@@ -4501,24 +4498,24 @@
         <v>1</v>
       </c>
       <c r="AI156" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="157" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE157">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AF157" t="s">
         <v>166</v>
       </c>
       <c r="AG157">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AH157">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AI157" t="s">
-        <v>19</v>
+        <v>54</v>
       </c>
     </row>
     <row r="158" spans="31:35" x14ac:dyDescent="0.2">
@@ -4526,33 +4523,33 @@
         <v>6</v>
       </c>
       <c r="AF158" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AG158">
         <v>6</v>
       </c>
       <c r="AH158">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AI158" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
     </row>
     <row r="159" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE159">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AF159" t="s">
         <v>167</v>
       </c>
       <c r="AG159">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AH159">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI159" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="160" spans="31:35" x14ac:dyDescent="0.2">
@@ -4560,16 +4557,16 @@
         <v>7</v>
       </c>
       <c r="AF160" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AG160">
         <v>7</v>
       </c>
       <c r="AH160">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AI160" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
     </row>
     <row r="161" spans="31:35" x14ac:dyDescent="0.2">
@@ -4577,47 +4574,47 @@
         <v>7</v>
       </c>
       <c r="AF161" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AG161">
         <v>7</v>
       </c>
       <c r="AH161">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="AI161" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="162" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE162">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AF162" t="s">
         <v>168</v>
       </c>
       <c r="AG162">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AH162">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="AI162" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="163" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE163">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AF163" t="s">
         <v>169</v>
       </c>
       <c r="AG163">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AH163">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AI163" t="s">
         <v>27</v>
@@ -4628,47 +4625,47 @@
         <v>9</v>
       </c>
       <c r="AF164" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AG164">
         <v>9</v>
       </c>
       <c r="AH164">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="AI164" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="165" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE165">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AF165" t="s">
         <v>170</v>
       </c>
       <c r="AG165">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AH165">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="AI165" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="166" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE166">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AF166" t="s">
         <v>171</v>
       </c>
       <c r="AG166">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AH166">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI166" t="s">
         <v>33</v>
@@ -4676,16 +4673,16 @@
     </row>
     <row r="167" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE167">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AF167" t="s">
         <v>172</v>
       </c>
       <c r="AG167">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AH167">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI167" t="s">
         <v>33</v>
@@ -4693,19 +4690,19 @@
     </row>
     <row r="168" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE168">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AF168" t="s">
         <v>173</v>
       </c>
       <c r="AG168">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AH168">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AI168" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="169" spans="31:35" x14ac:dyDescent="0.2">
@@ -4713,33 +4710,33 @@
         <v>13</v>
       </c>
       <c r="AF169" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AG169">
         <v>13</v>
       </c>
       <c r="AH169">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AI169" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="170" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE170">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AF170" t="s">
         <v>174</v>
       </c>
       <c r="AG170">
+        <v>14</v>
+      </c>
+      <c r="AH170">
+        <v>2</v>
+      </c>
+      <c r="AI170" t="s">
         <v>13</v>
-      </c>
-      <c r="AH170">
-        <v>4</v>
-      </c>
-      <c r="AI170" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="171" spans="31:35" x14ac:dyDescent="0.2">
@@ -4747,16 +4744,16 @@
         <v>14</v>
       </c>
       <c r="AF171" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AG171">
         <v>14</v>
       </c>
       <c r="AH171">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI171" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172" spans="31:35" x14ac:dyDescent="0.2">
@@ -4764,33 +4761,33 @@
         <v>14</v>
       </c>
       <c r="AF172" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AG172">
         <v>14</v>
       </c>
       <c r="AH172">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AI172" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="173" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE173">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AF173" t="s">
         <v>175</v>
       </c>
       <c r="AG173">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AH173">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AI173" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="174" spans="31:35" x14ac:dyDescent="0.2">
@@ -4798,7 +4795,7 @@
         <v>15</v>
       </c>
       <c r="AF174" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AG174">
         <v>15</v>
@@ -4807,24 +4804,24 @@
         <v>2</v>
       </c>
       <c r="AI174" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="175" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE175">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AF175" t="s">
         <v>176</v>
       </c>
       <c r="AG175">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AH175">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI175" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="176" spans="31:35" x14ac:dyDescent="0.2">
@@ -4832,33 +4829,33 @@
         <v>16</v>
       </c>
       <c r="AF176" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AG176">
         <v>16</v>
       </c>
       <c r="AH176">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AI176" t="s">
-        <v>39</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE177">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AF177" t="s">
-        <v>177</v>
+        <v>117</v>
       </c>
       <c r="AG177">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AH177">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="AI177" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
     </row>
     <row r="178" spans="31:35" x14ac:dyDescent="0.2">
@@ -4866,16 +4863,16 @@
         <v>17</v>
       </c>
       <c r="AF178" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG178">
         <v>17</v>
       </c>
       <c r="AH178">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AI178" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="179" spans="31:35" x14ac:dyDescent="0.2">
@@ -4883,16 +4880,16 @@
         <v>17</v>
       </c>
       <c r="AF179" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG179">
         <v>17</v>
       </c>
       <c r="AH179">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AI179" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="180" spans="31:35" x14ac:dyDescent="0.2">
@@ -4900,7 +4897,7 @@
         <v>17</v>
       </c>
       <c r="AF180" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG180">
         <v>17</v>
@@ -4909,7 +4906,7 @@
         <v>2</v>
       </c>
       <c r="AI180" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="181" spans="31:35" x14ac:dyDescent="0.2">
@@ -4917,16 +4914,16 @@
         <v>17</v>
       </c>
       <c r="AF181" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG181">
         <v>17</v>
       </c>
       <c r="AH181">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AI181" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="182" spans="31:35" x14ac:dyDescent="0.2">
@@ -4934,13 +4931,13 @@
         <v>17</v>
       </c>
       <c r="AF182" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG182">
         <v>17</v>
       </c>
       <c r="AH182">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AI182" t="s">
         <v>60</v>
@@ -4951,7 +4948,7 @@
         <v>17</v>
       </c>
       <c r="AF183" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG183">
         <v>17</v>
@@ -4960,7 +4957,7 @@
         <v>2</v>
       </c>
       <c r="AI183" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
     </row>
     <row r="184" spans="31:35" x14ac:dyDescent="0.2">
@@ -4968,7 +4965,7 @@
         <v>17</v>
       </c>
       <c r="AF184" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG184">
         <v>17</v>
@@ -4977,7 +4974,7 @@
         <v>2</v>
       </c>
       <c r="AI184" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="185" spans="31:35" x14ac:dyDescent="0.2">
@@ -4985,7 +4982,7 @@
         <v>17</v>
       </c>
       <c r="AF185" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG185">
         <v>17</v>
@@ -4994,7 +4991,7 @@
         <v>2</v>
       </c>
       <c r="AI185" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="186" spans="31:35" x14ac:dyDescent="0.2">
@@ -5002,7 +4999,7 @@
         <v>17</v>
       </c>
       <c r="AF186" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG186">
         <v>17</v>
@@ -5011,7 +5008,7 @@
         <v>2</v>
       </c>
       <c r="AI186" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="187" spans="31:35" x14ac:dyDescent="0.2">
@@ -5019,7 +5016,7 @@
         <v>17</v>
       </c>
       <c r="AF187" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG187">
         <v>17</v>
@@ -5028,7 +5025,7 @@
         <v>2</v>
       </c>
       <c r="AI187" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
     </row>
     <row r="188" spans="31:35" x14ac:dyDescent="0.2">
@@ -5036,16 +5033,16 @@
         <v>17</v>
       </c>
       <c r="AF188" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG188">
         <v>17</v>
       </c>
       <c r="AH188">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AI188" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="31:35" x14ac:dyDescent="0.2">
@@ -5053,16 +5050,16 @@
         <v>17</v>
       </c>
       <c r="AF189" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG189">
         <v>17</v>
       </c>
       <c r="AH189">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AI189" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
     </row>
     <row r="190" spans="31:35" x14ac:dyDescent="0.2">
@@ -5070,7 +5067,7 @@
         <v>17</v>
       </c>
       <c r="AF190" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG190">
         <v>17</v>
@@ -5079,7 +5076,7 @@
         <v>2</v>
       </c>
       <c r="AI190" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="191" spans="31:35" x14ac:dyDescent="0.2">
@@ -5087,7 +5084,7 @@
         <v>17</v>
       </c>
       <c r="AF191" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG191">
         <v>17</v>
@@ -5096,7 +5093,7 @@
         <v>2</v>
       </c>
       <c r="AI191" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="192" spans="31:35" x14ac:dyDescent="0.2">
@@ -5104,7 +5101,7 @@
         <v>17</v>
       </c>
       <c r="AF192" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG192">
         <v>17</v>
@@ -5113,24 +5110,24 @@
         <v>2</v>
       </c>
       <c r="AI192" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
     </row>
     <row r="193" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE193">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AF193" t="s">
-        <v>118</v>
+        <v>177</v>
       </c>
       <c r="AG193">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AH193">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="AI193" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="194" spans="31:35" x14ac:dyDescent="0.2">
@@ -5138,30 +5135,30 @@
         <v>18</v>
       </c>
       <c r="AF194" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AG194">
         <v>18</v>
       </c>
       <c r="AH194">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AI194" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="195" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE195">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AF195" t="s">
         <v>178</v>
       </c>
       <c r="AG195">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AH195">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI195" t="s">
         <v>41</v>
@@ -5169,19 +5166,19 @@
     </row>
     <row r="196" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE196">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AF196" t="s">
         <v>179</v>
       </c>
       <c r="AG196">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AH196">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AI196" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="197" spans="31:35" x14ac:dyDescent="0.2">
@@ -5189,33 +5186,33 @@
         <v>20</v>
       </c>
       <c r="AF197" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AG197">
         <v>20</v>
       </c>
       <c r="AH197">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AI197" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="198" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE198">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AF198" t="s">
         <v>180</v>
       </c>
       <c r="AG198">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AH198">
         <v>6</v>
       </c>
       <c r="AI198" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="199" spans="31:35" x14ac:dyDescent="0.2">
@@ -5223,33 +5220,33 @@
         <v>21</v>
       </c>
       <c r="AF199" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AG199">
         <v>21</v>
       </c>
       <c r="AH199">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AI199" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="200" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE200">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AF200" t="s">
         <v>181</v>
       </c>
       <c r="AG200">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AH200">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AI200" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="201" spans="31:35" x14ac:dyDescent="0.2">
@@ -5257,33 +5254,33 @@
         <v>22</v>
       </c>
       <c r="AF201" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AG201">
         <v>22</v>
       </c>
       <c r="AH201">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AI201" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="202" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE202">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AF202" t="s">
         <v>182</v>
       </c>
       <c r="AG202">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AH202">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AI202" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="203" spans="31:35" x14ac:dyDescent="0.2">
@@ -5291,33 +5288,33 @@
         <v>23</v>
       </c>
       <c r="AF203" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AG203">
         <v>23</v>
       </c>
       <c r="AH203">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="AI203" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="204" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE204">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AF204" t="s">
         <v>183</v>
       </c>
       <c r="AG204">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AH204">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="AI204" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="205" spans="31:35" x14ac:dyDescent="0.2">
@@ -5325,33 +5322,33 @@
         <v>24</v>
       </c>
       <c r="AF205" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG205">
         <v>24</v>
       </c>
       <c r="AH205">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AI205" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="206" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE206">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AF206" t="s">
         <v>184</v>
       </c>
       <c r="AG206">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AH206">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="AI206" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="207" spans="31:35" x14ac:dyDescent="0.2">
@@ -5359,30 +5356,30 @@
         <v>25</v>
       </c>
       <c r="AF207" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AG207">
         <v>25</v>
       </c>
       <c r="AH207">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="AI207" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="208" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE208">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AF208" t="s">
         <v>185</v>
       </c>
       <c r="AG208">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AH208">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AI208" t="s">
         <v>41</v>
@@ -5393,33 +5390,33 @@
         <v>26</v>
       </c>
       <c r="AF209" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AG209">
         <v>26</v>
       </c>
       <c r="AH209">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="AI209" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="210" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE210">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AF210" t="s">
         <v>186</v>
       </c>
       <c r="AG210">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AH210">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="AI210" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="211" spans="31:35" x14ac:dyDescent="0.2">
@@ -5427,16 +5424,16 @@
         <v>27</v>
       </c>
       <c r="AF211" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AG211">
         <v>27</v>
       </c>
       <c r="AH211">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="AI211" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="212" spans="31:35" x14ac:dyDescent="0.2">
@@ -5444,33 +5441,33 @@
         <v>27</v>
       </c>
       <c r="AF212" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AG212">
         <v>27</v>
       </c>
       <c r="AH212">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI212" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="213" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE213">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AF213" t="s">
         <v>187</v>
       </c>
       <c r="AG213">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AH213">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="AI213" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
     </row>
     <row r="214" spans="31:35" x14ac:dyDescent="0.2">
@@ -5478,16 +5475,16 @@
         <v>28</v>
       </c>
       <c r="AF214" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AG214">
         <v>28</v>
       </c>
       <c r="AH214">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="AI214" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="215" spans="31:35" x14ac:dyDescent="0.2">
@@ -5495,7 +5492,7 @@
         <v>28</v>
       </c>
       <c r="AF215" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="AG215">
         <v>28</v>
@@ -5504,24 +5501,24 @@
         <v>1</v>
       </c>
       <c r="AI215" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="216" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE216">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AF216" t="s">
         <v>188</v>
       </c>
       <c r="AG216">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AH216">
         <v>1</v>
       </c>
       <c r="AI216" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="217" spans="31:35" x14ac:dyDescent="0.2">
@@ -5529,50 +5526,50 @@
         <v>29</v>
       </c>
       <c r="AF217" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="AG217">
         <v>29</v>
       </c>
       <c r="AH217">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="AI217" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="218" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE218">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AF218" t="s">
         <v>189</v>
       </c>
       <c r="AG218">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AH218">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="AI218" t="s">
-        <v>41</v>
+        <v>60</v>
       </c>
     </row>
     <row r="219" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE219">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AF219" t="s">
         <v>190</v>
       </c>
       <c r="AG219">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AH219">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="AI219" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="220" spans="31:35" x14ac:dyDescent="0.2">
@@ -5580,13 +5577,13 @@
         <v>31</v>
       </c>
       <c r="AF220" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AG220">
         <v>31</v>
       </c>
       <c r="AH220">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AI220" t="s">
         <v>54</v>
@@ -5597,13 +5594,13 @@
         <v>31</v>
       </c>
       <c r="AF221" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AG221">
         <v>31</v>
       </c>
       <c r="AH221">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AI221" t="s">
         <v>54</v>
@@ -5614,16 +5611,16 @@
         <v>31</v>
       </c>
       <c r="AF222" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AG222">
         <v>31</v>
       </c>
       <c r="AH222">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="AI222" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="223" spans="31:35" x14ac:dyDescent="0.2">
@@ -5631,13 +5628,13 @@
         <v>31</v>
       </c>
       <c r="AF223" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AG223">
         <v>31</v>
       </c>
       <c r="AH223">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="AI223" t="s">
         <v>60</v>
@@ -5648,16 +5645,16 @@
         <v>31</v>
       </c>
       <c r="AF224" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AG224">
         <v>31</v>
       </c>
       <c r="AH224">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="AI224" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="225" spans="31:35" x14ac:dyDescent="0.2">
@@ -5665,13 +5662,13 @@
         <v>31</v>
       </c>
       <c r="AF225" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AG225">
         <v>31</v>
       </c>
       <c r="AH225">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AI225" t="s">
         <v>54</v>
@@ -5682,13 +5679,13 @@
         <v>31</v>
       </c>
       <c r="AF226" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AG226">
         <v>31</v>
       </c>
       <c r="AH226">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="AI226" t="s">
         <v>54</v>
@@ -5699,13 +5696,13 @@
         <v>31</v>
       </c>
       <c r="AF227" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AG227">
         <v>31</v>
       </c>
       <c r="AH227">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AI227" t="s">
         <v>54</v>
@@ -5716,13 +5713,13 @@
         <v>31</v>
       </c>
       <c r="AF228" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AG228">
         <v>31</v>
       </c>
       <c r="AH228">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AI228" t="s">
         <v>54</v>
@@ -5733,13 +5730,13 @@
         <v>31</v>
       </c>
       <c r="AF229" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AG229">
         <v>31</v>
       </c>
       <c r="AH229">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AI229" t="s">
         <v>54</v>
@@ -5750,13 +5747,13 @@
         <v>31</v>
       </c>
       <c r="AF230" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AG230">
         <v>31</v>
       </c>
       <c r="AH230">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AI230" t="s">
         <v>54</v>
@@ -5764,36 +5761,36 @@
     </row>
     <row r="231" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE231">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AF231" t="s">
         <v>191</v>
       </c>
       <c r="AG231">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AH231">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="AI231" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="232" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE232">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AF232" t="s">
         <v>192</v>
       </c>
       <c r="AG232">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AH232">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="AI232" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
     </row>
     <row r="233" spans="31:35" x14ac:dyDescent="0.2">
@@ -5801,16 +5798,16 @@
         <v>33</v>
       </c>
       <c r="AF233" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AG233">
         <v>33</v>
       </c>
       <c r="AH233">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AI233" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
     </row>
     <row r="234" spans="31:35" x14ac:dyDescent="0.2">
@@ -5818,33 +5815,33 @@
         <v>33</v>
       </c>
       <c r="AF234" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="AG234">
         <v>33</v>
       </c>
       <c r="AH234">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AI234" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="235" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE235">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AF235" t="s">
         <v>193</v>
       </c>
       <c r="AG235">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AH235">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AI235" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
     </row>
     <row r="236" spans="31:35" x14ac:dyDescent="0.2">
@@ -5852,16 +5849,16 @@
         <v>34</v>
       </c>
       <c r="AF236" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AG236">
         <v>34</v>
       </c>
       <c r="AH236">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AI236" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
     </row>
     <row r="237" spans="31:35" x14ac:dyDescent="0.2">
@@ -5869,16 +5866,16 @@
         <v>34</v>
       </c>
       <c r="AF237" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AG237">
         <v>34</v>
       </c>
       <c r="AH237">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AI237" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="238" spans="31:35" x14ac:dyDescent="0.2">
@@ -5886,7 +5883,7 @@
         <v>34</v>
       </c>
       <c r="AF238" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AG238">
         <v>34</v>
@@ -5895,24 +5892,24 @@
         <v>1</v>
       </c>
       <c r="AI238" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="239" spans="31:35" x14ac:dyDescent="0.2">
       <c r="AE239">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AF239" t="s">
         <v>194</v>
       </c>
       <c r="AG239">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AH239">
         <v>1</v>
       </c>
       <c r="AI239" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="240" spans="31:35" x14ac:dyDescent="0.2">
@@ -5920,38 +5917,21 @@
         <v>35</v>
       </c>
       <c r="AF240" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="AG240">
         <v>35</v>
       </c>
       <c r="AH240">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AI240" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="241" spans="31:35" x14ac:dyDescent="0.2">
-      <c r="AE241">
-        <v>35</v>
-      </c>
-      <c r="AF241" t="s">
-        <v>195</v>
-      </c>
-      <c r="AG241">
-        <v>35</v>
-      </c>
-      <c r="AH241">
-        <v>3</v>
-      </c>
-      <c r="AI241" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:AT267">
-    <sortCondition ref="A1:A267"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:AT266">
+    <sortCondition ref="A1:A266"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>